<commit_message>
Added new instruction set file
</commit_message>
<xml_diff>
--- a/InstructionSet.xlsx
+++ b/InstructionSet.xlsx
@@ -2,23 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnu\Google Drive\AAU\P4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnu\Documents\Git\EIT-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B9EE19-ADE5-48E0-80A5-16CD27F6D7FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D84CBE5-A659-4EC0-830C-DD91D1931073}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="8100" activeTab="2" xr2:uid="{71A0F77E-B2EC-49EE-B056-41294540D1EE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" firstSheet="1" activeTab="2" xr2:uid="{7153551F-15F7-4547-9B59-5230311ACC28}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
     <sheet name="Instruction Set 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="117">
   <si>
     <t>Control Signals</t>
   </si>
@@ -279,6 +280,108 @@
   </si>
   <si>
     <t>ORR</t>
+  </si>
+  <si>
+    <t>HALT</t>
+  </si>
+  <si>
+    <t>34420001</t>
+  </si>
+  <si>
+    <t>Add 1 to R2</t>
+  </si>
+  <si>
+    <t>Store R2 in location R5</t>
+  </si>
+  <si>
+    <t>98000000</t>
+  </si>
+  <si>
+    <t>JMPNQ</t>
+  </si>
+  <si>
+    <t>If not equal jump to 3</t>
+  </si>
+  <si>
+    <t>94000003</t>
+  </si>
+  <si>
+    <t>741AFDE9</t>
+  </si>
+  <si>
+    <t>Move 65001 into r26</t>
+  </si>
+  <si>
+    <t>7CA20000</t>
+  </si>
+  <si>
+    <t>Move 1F into R25</t>
+  </si>
+  <si>
+    <t>7F590000</t>
+  </si>
+  <si>
+    <t>Store R25 in location R26</t>
+  </si>
+  <si>
+    <t>7419001F</t>
+  </si>
+  <si>
+    <t>7405FDE8</t>
+  </si>
+  <si>
+    <t>Move 65000 into R5</t>
+  </si>
+  <si>
+    <t>Compare R2 to 5000</t>
+  </si>
+  <si>
+    <t>70401388</t>
+  </si>
+  <si>
+    <t>PUSH PC</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>POP PC</t>
+  </si>
+  <si>
+    <t>854AF800</t>
+  </si>
+  <si>
+    <t>814A07C0</t>
+  </si>
+  <si>
+    <t>7B580000</t>
+  </si>
+  <si>
+    <t>Load location R26 into R24</t>
+  </si>
+  <si>
+    <t>854AC000</t>
+  </si>
+  <si>
+    <t>PUSH R24</t>
+  </si>
+  <si>
+    <t>POP to R23</t>
+  </si>
+  <si>
+    <t>ADD 4 to R23</t>
+  </si>
+  <si>
+    <t>814A05C0</t>
+  </si>
+  <si>
+    <t>36F70004</t>
+  </si>
+  <si>
+    <t>741A0100</t>
+  </si>
+  <si>
+    <t>Move 256 into r26</t>
   </si>
 </sst>
 </file>
@@ -337,10 +440,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,6 +470,7 @@
       <sheetName val="FunctionsBook"/>
       <sheetName val="CommandBarMenu"/>
       <sheetName val="setting"/>
+      <sheetName val="XN"/>
     </sheetNames>
     <definedNames>
       <definedName name="cvBinDec"/>
@@ -378,6 +482,7 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -680,21 +785,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2F1AFC-A2B0-4C4C-904C-A9FB789B0FD8}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="34" max="37" width="9.28515625" customWidth="1"/>
+    <col min="2" max="3" width="15.3984375" customWidth="1"/>
+    <col min="34" max="37" width="9.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -807,7 +910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -914,7 +1017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1021,7 +1124,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1128,11 +1231,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
@@ -1171,40 +1274,40 @@
       <c r="O5" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="X5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="Y5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="Z5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="6" t="s">
+      <c r="AA5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AB5" s="6" t="s">
+      <c r="AB5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AC5" s="3"/>
@@ -1217,32 +1320,32 @@
       <c r="AG5" t="s">
         <v>42</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AI5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AL5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AM5" s="6" t="s">
+      <c r="AM5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AN5" s="4"/>
-      <c r="AO5" s="6"/>
+      <c r="AO5" s="7"/>
       <c r="AP5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ5" s="6" t="s">
+      <c r="AQ5" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="D6" t="s">
         <v>42</v>
       </c>
@@ -1279,18 +1382,18 @@
       <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
       <c r="AC6" s="3"/>
       <c r="AD6" t="s">
         <v>42</v>
@@ -1301,22 +1404,22 @@
       <c r="AG6" t="s">
         <v>42</v>
       </c>
-      <c r="AI6" s="6"/>
-      <c r="AJ6" s="6"/>
-      <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
       <c r="AN6" s="4"/>
-      <c r="AO6" s="6"/>
+      <c r="AO6" s="7"/>
       <c r="AP6" t="s">
         <v>42</v>
       </c>
-      <c r="AQ6" s="6"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="7"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -1353,18 +1456,18 @@
       <c r="O7" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
       <c r="AC7" s="3"/>
       <c r="AD7" t="s">
         <v>42</v>
@@ -1375,25 +1478,25 @@
       <c r="AG7" t="s">
         <v>42</v>
       </c>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-      <c r="AL7" s="6"/>
-      <c r="AM7" s="6"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
       <c r="AN7" s="4"/>
-      <c r="AO7" s="6"/>
+      <c r="AO7" s="7"/>
       <c r="AP7" t="s">
         <v>63</v>
       </c>
-      <c r="AQ7" s="6"/>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="7"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1607,7 +1710,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1714,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1821,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2142,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2251,12 +2354,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AA5:AA7"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AM5:AM7"/>
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AO5:AO7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="Q5:Q7"/>
     <mergeCell ref="R5:R7"/>
@@ -2270,6 +2367,12 @@
     <mergeCell ref="AJ5:AJ7"/>
     <mergeCell ref="Y5:Y7"/>
     <mergeCell ref="Z5:Z7"/>
+    <mergeCell ref="AA5:AA7"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="AI5:AI7"/>
+    <mergeCell ref="AM5:AM7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AO5:AO7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2278,21 +2381,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8889DF25-7328-4608-ADDC-50AC9A76EA77}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView topLeftCell="R1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="34" max="37" width="9.28515625" customWidth="1"/>
+    <col min="2" max="3" width="15.3984375" customWidth="1"/>
+    <col min="34" max="37" width="9.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -2405,7 +2506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2515,7 +2616,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2625,7 +2726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -2735,11 +2836,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
@@ -2778,40 +2879,40 @@
       <c r="O5" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="X5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="Y5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="Z5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="6" t="s">
+      <c r="AA5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AB5" s="6" t="s">
+      <c r="AB5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AC5" s="5"/>
@@ -2824,16 +2925,16 @@
       <c r="AG5" t="s">
         <v>42</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AI5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AL5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AM5" s="6" t="s">
+      <c r="AM5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="AN5" s="5"/>
@@ -2843,15 +2944,15 @@
       <c r="AP5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ5" s="6" t="s">
+      <c r="AQ5" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="D6" t="s">
         <v>42</v>
       </c>
@@ -2888,18 +2989,18 @@
       <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
       <c r="AC6" s="5"/>
       <c r="AD6" t="s">
         <v>42</v>
@@ -2910,10 +3011,10 @@
       <c r="AG6" t="s">
         <v>42</v>
       </c>
-      <c r="AI6" s="6"/>
-      <c r="AJ6" s="6"/>
-      <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
       <c r="AN6" s="5"/>
       <c r="AO6" t="s">
         <v>34</v>
@@ -2921,13 +3022,13 @@
       <c r="AP6" t="s">
         <v>42</v>
       </c>
-      <c r="AQ6" s="6"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="7"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -2964,18 +3065,18 @@
       <c r="O7" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
       <c r="AC7" s="5"/>
       <c r="AD7" t="s">
         <v>42</v>
@@ -2986,10 +3087,10 @@
       <c r="AG7" t="s">
         <v>42</v>
       </c>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-      <c r="AL7" s="6"/>
-      <c r="AM7" s="6"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
       <c r="AN7" s="5"/>
       <c r="AO7" t="s">
         <v>23</v>
@@ -2997,16 +3098,16 @@
       <c r="AP7" t="s">
         <v>63</v>
       </c>
-      <c r="AQ7" s="6"/>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="7"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -3122,7 +3223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3238,7 +3339,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3354,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -3470,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3586,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3702,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -3818,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -3936,12 +4037,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AJ5:AJ7"/>
-    <mergeCell ref="AL5:AL7"/>
-    <mergeCell ref="AM5:AM7"/>
     <mergeCell ref="AA5:AA7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="Q5:Q7"/>
@@ -3954,6 +4049,12 @@
     <mergeCell ref="X5:X7"/>
     <mergeCell ref="Y5:Y7"/>
     <mergeCell ref="Z5:Z7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="AI5:AI7"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="AL5:AL7"/>
+    <mergeCell ref="AM5:AM7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3961,272 +4062,274 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD26F98B-7A30-41DA-ABC7-DF54B76441DB}">
-  <dimension ref="A1:U37"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="3" max="3" width="37.265625" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C1" t="str">
-        <f>DEC2BIN(VLOOKUP(B1,T1:U37,2,FALSE),6)</f>
-        <v>000001</v>
-      </c>
-      <c r="T1" t="s">
+        <f>DEC2BIN(VLOOKUP(B1,G1:H38,2,FALSE),6)</f>
+        <v>011110</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2BIN(B2,5)</f>
-        <v>01000</v>
-      </c>
-      <c r="T2" t="s">
+        <v>11010</v>
+      </c>
+      <c r="G2" t="s">
         <v>73</v>
       </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3" si="0">DEC2BIN(B3,5)</f>
-        <v>01000</v>
-      </c>
-      <c r="T3" t="s">
+        <v>11000</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="U3">
+      <c r="H3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4" t="str">
         <f>DEC2BIN(MOD(QUOTIENT($B$4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($B$4,256^0),256),8)</f>
-        <v>0000000000001000</v>
-      </c>
-      <c r="T4" t="s">
+        <v>0000000000000000</v>
+      </c>
+      <c r="G4" t="s">
         <v>74</v>
       </c>
-      <c r="U4">
+      <c r="H4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="T5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="7"/>
+      <c r="G5" t="s">
         <v>75</v>
       </c>
-      <c r="U5">
+      <c r="H5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="T6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="7"/>
+      <c r="G6" t="s">
         <v>76</v>
       </c>
-      <c r="U6">
+      <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
         <v>82</v>
       </c>
-      <c r="U7">
+      <c r="H7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C8" t="str">
         <f>C1&amp;C2&amp;C3&amp;C4</f>
-        <v>00000101000010000000000000001000</v>
+        <v>01111011010110000000000000000000</v>
       </c>
       <c r="E8" t="str">
         <f>[1]!cvDecBase([1]!cvBinDec(C8),16)</f>
-        <v>5080008</v>
-      </c>
-      <c r="T8" t="s">
+        <v>7B580000</v>
+      </c>
+      <c r="G8" t="s">
         <v>77</v>
       </c>
-      <c r="U8">
+      <c r="H8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T9" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="U9">
+      <c r="H9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
         <v>78</v>
       </c>
-      <c r="U10">
+      <c r="H10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
       <c r="L11" t="str">
         <f>L4&amp;L5&amp;L6&amp;L7</f>
         <v/>
       </c>
-      <c r="T11" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T12" t="s">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
         <v>80</v>
       </c>
-      <c r="U12">
+      <c r="H12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
         <v>81</v>
       </c>
-      <c r="U13">
+      <c r="H13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C14" t="str">
-        <f>DEC2BIN(VLOOKUP(B14,T1:U37,2,FALSE),6)</f>
-        <v>000011</v>
-      </c>
-      <c r="T14" t="s">
+        <f>DEC2BIN(VLOOKUP(B14,G1:H37,2,FALSE),6)</f>
+        <v>100000</v>
+      </c>
+      <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="U14">
+      <c r="H14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" t="str">
         <f>DEC2BIN(B15,5)</f>
-        <v>01000</v>
-      </c>
-      <c r="T15" t="s">
+        <v>01010</v>
+      </c>
+      <c r="G15" t="s">
         <v>48</v>
       </c>
-      <c r="U15">
+      <c r="H15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ref="C16:C18" si="1">DEC2BIN(B16,5)</f>
-        <v>01000</v>
-      </c>
-      <c r="T16" t="s">
+        <v>01010</v>
+      </c>
+      <c r="G16" t="s">
         <v>49</v>
       </c>
-      <c r="U16">
+      <c r="H16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
-        <v>01000</v>
-      </c>
-      <c r="T17" t="s">
+        <v>00000</v>
+      </c>
+      <c r="G17" t="s">
         <v>50</v>
       </c>
-      <c r="U17">
+      <c r="H17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
-        <v>01000</v>
-      </c>
-      <c r="T18" t="s">
+        <v>00000</v>
+      </c>
+      <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="U18">
+      <c r="H18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -4237,166 +4340,174 @@
         <f>DEC2BIN(B19,6)</f>
         <v>000000</v>
       </c>
-      <c r="T19" t="s">
+      <c r="G19" t="s">
         <v>52</v>
       </c>
-      <c r="U19">
+      <c r="H19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T20" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
         <v>53</v>
       </c>
-      <c r="U20">
+      <c r="H20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C21" t="str">
         <f>C14&amp;C15&amp;C16&amp;C17&amp;C18&amp;C19</f>
-        <v>00001101000010000100001000000000</v>
-      </c>
-      <c r="E21" t="str">
-        <f>[1]!cvDecBase([1]!cvBinDec(C21),16)</f>
-        <v>D084200</v>
-      </c>
-      <c r="T21" t="s">
+        <v>10000001010010100000000000000000</v>
+      </c>
+      <c r="E21" t="e">
+        <f ca="1">[1]!cvDecBase([1]!cvBinDec(C21),16)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="U21">
+      <c r="H21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T22" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
         <v>43</v>
       </c>
-      <c r="U22">
+      <c r="H22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T23" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
         <v>44</v>
       </c>
-      <c r="U23">
+      <c r="H23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T24" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
         <v>45</v>
       </c>
-      <c r="U24">
+      <c r="H24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T25" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
         <v>46</v>
       </c>
-      <c r="U25">
+      <c r="H25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T26" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
         <v>12</v>
       </c>
-      <c r="U26">
+      <c r="H26">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T27" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
         <v>18</v>
       </c>
-      <c r="U27">
+      <c r="H27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T28" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
         <v>57</v>
       </c>
-      <c r="U28">
+      <c r="H28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T29" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
         <v>58</v>
       </c>
-      <c r="U29">
+      <c r="H29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T30" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
         <v>19</v>
       </c>
-      <c r="U30">
+      <c r="H30">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T31" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
         <v>20</v>
       </c>
-      <c r="U31">
+      <c r="H31">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T32" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G32" t="s">
         <v>21</v>
       </c>
-      <c r="U32">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T33" t="s">
+      <c r="H32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G33" t="s">
         <v>22</v>
       </c>
-      <c r="U33">
+      <c r="H33">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T34" t="s">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G34" t="s">
         <v>28</v>
       </c>
-      <c r="U34">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T35" t="s">
+      <c r="H34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
         <v>29</v>
       </c>
-      <c r="U35">
+      <c r="H35">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T36" t="s">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
         <v>30</v>
       </c>
-      <c r="U36">
+      <c r="H36">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="20:21" x14ac:dyDescent="0.25">
-      <c r="T37" t="s">
-        <v>31</v>
-      </c>
-      <c r="U37">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37">
         <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4406,4 +4517,371 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B22A9C-F797-407A-A147-CBC83D093D8A}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="27.73046875" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" customWidth="1"/>
+    <col min="14" max="14" width="24.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>88000005</v>
+      </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made progress on interrupts. Fixed bug where mem was continiously writte
</commit_message>
<xml_diff>
--- a/InstructionSet.xlsx
+++ b/InstructionSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnu\Documents\Git\EIT-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D84CBE5-A659-4EC0-830C-DD91D1931073}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96CAB7CB-D1CF-497A-9360-96A382A13B68}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" firstSheet="1" activeTab="2" xr2:uid="{7153551F-15F7-4547-9B59-5230311ACC28}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" firstSheet="1" activeTab="3" xr2:uid="{7153551F-15F7-4547-9B59-5230311ACC28}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="110">
   <si>
     <t>Control Signals</t>
   </si>
@@ -339,49 +339,28 @@
     <t>70401388</t>
   </si>
   <si>
-    <t>PUSH PC</t>
-  </si>
-  <si>
-    <t>JUMP</t>
-  </si>
-  <si>
-    <t>POP PC</t>
-  </si>
-  <si>
-    <t>854AF800</t>
-  </si>
-  <si>
-    <t>814A07C0</t>
-  </si>
-  <si>
-    <t>7B580000</t>
-  </si>
-  <si>
-    <t>Load location R26 into R24</t>
-  </si>
-  <si>
-    <t>854AC000</t>
-  </si>
-  <si>
-    <t>PUSH R24</t>
-  </si>
-  <si>
-    <t>POP to R23</t>
-  </si>
-  <si>
-    <t>ADD 4 to R23</t>
-  </si>
-  <si>
-    <t>814A05C0</t>
-  </si>
-  <si>
-    <t>36F70004</t>
-  </si>
-  <si>
-    <t>741A0100</t>
-  </si>
-  <si>
-    <t>Move 256 into r26</t>
+    <t>74190066</t>
+  </si>
+  <si>
+    <t>MOVE 102 into R25</t>
+  </si>
+  <si>
+    <t>741AFE4C</t>
+  </si>
+  <si>
+    <t>MOVE 65100 into R26</t>
+  </si>
+  <si>
+    <t>MOVE 103 into R25</t>
+  </si>
+  <si>
+    <t>MOVE 65101 into R26</t>
+  </si>
+  <si>
+    <t>741AFE4D</t>
+  </si>
+  <si>
+    <t>9400000C</t>
   </si>
 </sst>
 </file>
@@ -470,7 +449,6 @@
       <sheetName val="FunctionsBook"/>
       <sheetName val="CommandBarMenu"/>
       <sheetName val="setting"/>
-      <sheetName val="XN"/>
     </sheetNames>
     <definedNames>
       <definedName name="cvBinDec"/>
@@ -482,7 +460,6 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -790,14 +767,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="3" width="15.3984375" customWidth="1"/>
-    <col min="34" max="37" width="9.265625" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
+    <col min="34" max="37" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -910,7 +887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +994,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1101,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1231,7 +1208,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1341,7 +1318,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1392,7 @@
       </c>
       <c r="AQ6" s="7"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -1489,14 +1466,14 @@
       </c>
       <c r="AQ7" s="7"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1603,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +1687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1817,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1924,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2138,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2245,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2354,6 +2331,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AM5:AM7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AO5:AO7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="Q5:Q7"/>
     <mergeCell ref="R5:R7"/>
@@ -2370,9 +2350,6 @@
     <mergeCell ref="AA5:AA7"/>
     <mergeCell ref="AB5:AB7"/>
     <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AM5:AM7"/>
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AO5:AO7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2386,14 +2363,14 @@
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="3" width="15.3984375" customWidth="1"/>
-    <col min="34" max="37" width="9.265625" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
+    <col min="34" max="37" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -2506,7 +2483,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2616,7 +2593,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2726,7 +2703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -2836,7 +2813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2948,7 +2925,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -3024,7 +3001,7 @@
       </c>
       <c r="AQ6" s="7"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -3100,14 +3077,14 @@
       </c>
       <c r="AQ7" s="7"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -3223,7 +3200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3339,7 +3316,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3455,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -3571,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3687,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3803,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -3919,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -4037,6 +4014,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="AI5:AI7"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="AL5:AL7"/>
+    <mergeCell ref="AM5:AM7"/>
     <mergeCell ref="AA5:AA7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="Q5:Q7"/>
@@ -4049,12 +4032,6 @@
     <mergeCell ref="X5:X7"/>
     <mergeCell ref="Y5:Y7"/>
     <mergeCell ref="Z5:Z7"/>
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AJ5:AJ7"/>
-    <mergeCell ref="AL5:AL7"/>
-    <mergeCell ref="AM5:AM7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4065,29 +4042,29 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
-    <col min="3" max="3" width="37.265625" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C1" t="str">
         <f>DEC2BIN(VLOOKUP(B1,G1:H38,2,FALSE),6)</f>
-        <v>011110</v>
+        <v>011101</v>
       </c>
       <c r="G1" t="s">
         <v>23</v>
@@ -4096,16 +4073,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2BIN(B2,5)</f>
-        <v>11010</v>
+        <v>00000</v>
       </c>
       <c r="G2" t="s">
         <v>73</v>
@@ -4114,16 +4091,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3" si="0">DEC2BIN(B3,5)</f>
-        <v>11000</v>
+        <v>11010</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -4132,16 +4109,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>65100</v>
       </c>
       <c r="C4" t="str">
         <f>DEC2BIN(MOD(QUOTIENT($B$4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($B$4,256^0),256),8)</f>
-        <v>0000000000000000</v>
+        <v>1111111001001100</v>
       </c>
       <c r="G4" t="s">
         <v>74</v>
@@ -4150,7 +4127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="G5" t="s">
         <v>75</v>
@@ -4159,7 +4136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="G6" t="s">
         <v>76</v>
@@ -4168,7 +4145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>82</v>
       </c>
@@ -4176,17 +4153,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C8" t="str">
         <f>C1&amp;C2&amp;C3&amp;C4</f>
-        <v>01111011010110000000000000000000</v>
+        <v>01110100000110101111111001001100</v>
       </c>
       <c r="E8" t="str">
         <f>[1]!cvDecBase([1]!cvBinDec(C8),16)</f>
-        <v>7B580000</v>
+        <v>741AFE4C</v>
       </c>
       <c r="G8" t="s">
         <v>77</v>
@@ -4195,7 +4172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>27</v>
       </c>
@@ -4203,7 +4180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>78</v>
       </c>
@@ -4211,7 +4188,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>79</v>
       </c>
@@ -4223,7 +4200,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
         <v>80</v>
       </c>
@@ -4231,7 +4208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>81</v>
       </c>
@@ -4239,7 +4216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -4257,7 +4234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4275,7 +4252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -4293,7 +4270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -4311,16 +4288,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
-        <v>00000</v>
+        <v>10111</v>
       </c>
       <c r="G18" t="s">
         <v>51</v>
@@ -4329,7 +4306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -4347,7 +4324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>53</v>
       </c>
@@ -4355,17 +4332,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C21" t="str">
         <f>C14&amp;C15&amp;C16&amp;C17&amp;C18&amp;C19</f>
-        <v>10000001010010100000000000000000</v>
-      </c>
-      <c r="E21" t="e">
-        <f ca="1">[1]!cvDecBase([1]!cvBinDec(C21),16)</f>
-        <v>#NAME?</v>
+        <v>10000001010010100000010111000000</v>
+      </c>
+      <c r="E21" t="str">
+        <f>[1]!cvDecBase([1]!cvBinDec(C21),16)</f>
+        <v>814A05C0</v>
       </c>
       <c r="G21" t="s">
         <v>54</v>
@@ -4374,7 +4351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>43</v>
       </c>
@@ -4382,7 +4359,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>44</v>
       </c>
@@ -4390,7 +4367,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>45</v>
       </c>
@@ -4398,7 +4375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>46</v>
       </c>
@@ -4406,7 +4383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>12</v>
       </c>
@@ -4414,7 +4391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
         <v>18</v>
       </c>
@@ -4422,7 +4399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
         <v>57</v>
       </c>
@@ -4430,7 +4407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>58</v>
       </c>
@@ -4438,7 +4415,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
         <v>19</v>
       </c>
@@ -4446,7 +4423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>20</v>
       </c>
@@ -4454,7 +4431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>21</v>
       </c>
@@ -4462,7 +4439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>22</v>
       </c>
@@ -4470,7 +4447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>28</v>
       </c>
@@ -4478,7 +4455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
         <v>29</v>
       </c>
@@ -4486,7 +4463,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
         <v>30</v>
       </c>
@@ -4494,7 +4471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>88</v>
       </c>
@@ -4502,7 +4479,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
         <v>83</v>
       </c>
@@ -4522,22 +4499,22 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B22A9C-F797-407A-A147-CBC83D093D8A}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.86328125" customWidth="1"/>
-    <col min="2" max="2" width="27.73046875" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" customWidth="1"/>
-    <col min="10" max="10" width="26.73046875" customWidth="1"/>
-    <col min="14" max="14" width="24.1328125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -4556,14 +4533,8 @@
       <c r="J1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -4582,14 +4553,8 @@
       <c r="J2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -4608,14 +4573,8 @@
       <c r="J3" t="s">
         <v>99</v>
       </c>
-      <c r="M3" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4634,14 +4593,8 @@
       <c r="J4" t="s">
         <v>96</v>
       </c>
-      <c r="M4" t="s">
-        <v>107</v>
-      </c>
-      <c r="N4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -4655,19 +4608,13 @@
         <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="M5" t="s">
-        <v>109</v>
-      </c>
-      <c r="N5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -4680,20 +4627,14 @@
       <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="I6">
-        <v>88000005</v>
+      <c r="I6" t="s">
+        <v>104</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -4707,19 +4648,13 @@
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>100</v>
-      </c>
-      <c r="M7" t="s">
-        <v>114</v>
-      </c>
-      <c r="N7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -4732,20 +4667,14 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
-        <v>90</v>
+      <c r="I8">
+        <v>74190067</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -4759,45 +4688,69 @@
         <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="I10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>84</v>
       </c>
       <c r="F11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>101</v>
       </c>
       <c r="F13" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>90</v>
       </c>
@@ -4811,7 +4764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>87</v>
       </c>
@@ -4825,7 +4778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I16">
         <v>0</v>
       </c>
@@ -4833,52 +4786,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.45">
-      <c r="I17">
-        <v>0</v>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>84</v>
       </c>
       <c r="J17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.45">
-      <c r="I18">
-        <v>0</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>93</v>
       </c>
       <c r="J18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.45">
-      <c r="I19">
-        <v>0</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>101</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.45">
-      <c r="I22" t="s">
-        <v>106</v>
-      </c>
-      <c r="J22" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>